<commit_message>
Cambios name Data Tracking
Cambios name Data Tracking
</commit_message>
<xml_diff>
--- a/public/uploads/invoice/invoice-6.xlsx
+++ b/public/uploads/invoice/invoice-6.xlsx
@@ -35,7 +35,7 @@
     <t>Office: 404-684-5963</t>
   </si>
   <si>
-    <t>24/04/2024</t>
+    <t>26/04/2024</t>
   </si>
   <si>
     <t>East Point, Ga. 30344</t>
@@ -1332,7 +1332,7 @@
   <dimension ref="A1:L205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="false" showRowColHeaders="1" topLeftCell="A10">
-      <selection activeCell="H26" sqref="H26:I26"/>
+      <selection activeCell="H27" sqref="H27:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="true" defaultRowHeight="15" defaultColWidth="8.88671875" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1736,7 +1736,7 @@
         <v>45</v>
       </c>
       <c r="F24" s="91">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="G24" s="91">
         <v>16.5</v>
@@ -1759,28 +1759,36 @@
         <v>47</v>
       </c>
       <c r="F25" s="91">
-        <v>20</v>
+        <v>20.0</v>
       </c>
       <c r="G25" s="91">
-        <v>58</v>
+        <v>58.0</v>
       </c>
       <c r="H25" s="92">
-        <v>1160</v>
+        <v>1160.0</v>
       </c>
       <c r="I25" s="93"/>
     </row>
     <row r="26" spans="1:12" customHeight="1" ht="15">
-      <c r="A26" s="85"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="85"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="94" t="s">
-        <v>48</v>
+      <c r="A26" s="87">
+        <v>3</v>
+      </c>
+      <c r="B26" s="88" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="89"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="87" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="91">
+        <v>1000.0</v>
+      </c>
+      <c r="G26" s="91">
+        <v>58.0</v>
       </c>
       <c r="H26" s="92">
-        <v>2810.0</v>
+        <v>58000.0</v>
       </c>
       <c r="I26" s="93"/>
     </row>
@@ -1791,9 +1799,13 @@
       <c r="D27" s="30"/>
       <c r="E27" s="85"/>
       <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="86"/>
-      <c r="I27" s="86"/>
+      <c r="G27" s="94" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" s="92">
+        <v>60810.0</v>
+      </c>
+      <c r="I27" s="93"/>
     </row>
     <row r="28" spans="1:12" customHeight="1" ht="15">
       <c r="A28" s="85"/>

</xml_diff>